<commit_message>
merchantID de base en el frontend
</commit_message>
<xml_diff>
--- a/subaccounts.xlsx
+++ b/subaccounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Personal\Documentos personales\SCRIPT\Onboarding-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31B4997-87B9-49EE-8D86-035CD9570DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E322C750-4B79-4B64-B141-295C5A8D35D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{12373DC2-E3C6-41F0-A981-02CBE3560ADC}"/>
   </bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>clientId</t>
-  </si>
-  <si>
-    <t>merchantId</t>
   </si>
   <si>
     <t>merchantSiteId</t>
@@ -417,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C1007B-24F9-43FF-9CE1-D1FD768442E8}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -425,16 +422,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -448,13 +444,10 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>